<commit_message>
test voltage and current reading
</commit_message>
<xml_diff>
--- a/testing/manual test log.xlsx
+++ b/testing/manual test log.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/dtey002_e_ntu_edu_sg/Documents/School/Modules/Y3S1/TMJN10 Software Engineering Project Methods/testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/dtey002_e_ntu_edu_sg/Documents/School/Modules/Y3S1/TMJN10 Software Engineering Project Methods/FlexiCharge-BMS/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6CAB6B7-631D-4F22-B51F-1583AEAFFA80}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C88DFF6C-D52E-494A-B1BD-2D1560D127D3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18915" windowHeight="11956" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Commit #" sheetId="1" r:id="rId1"/>
+    <sheet name="Issue #36, #74" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,9 +66,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Expected Output</t>
   </si>
   <si>
@@ -78,15 +75,6 @@
     <t>Deviation</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Test of voltage reading of individual cells</t>
-  </si>
-  <si>
-    <t>Commit #</t>
-  </si>
-  <si>
     <t>Maximum Deviation</t>
   </si>
   <si>
@@ -111,7 +99,19 @@
     <t>Test #</t>
   </si>
   <si>
-    <t>Test of current reading</t>
+    <t>Issue #</t>
+  </si>
+  <si>
+    <t>Input (V)</t>
+  </si>
+  <si>
+    <t>Test of voltage reading of individual cells. Input measurement error ~0.01V</t>
+  </si>
+  <si>
+    <t>Input (mA)</t>
+  </si>
+  <si>
+    <t>Test of current reading. Input measurement error ~5mA</t>
   </si>
 </sst>
 </file>
@@ -209,16 +209,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,11 +226,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -249,11 +250,6 @@
     <dxf>
       <font>
         <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
       </font>
     </dxf>
   </dxfs>
@@ -534,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -549,75 +545,83 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
+      <c r="C2" s="8">
+        <v>45197</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2">
+        <v>74</v>
+      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="4" t="s">
-        <v>16</v>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="J4" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="I5" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="I5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
@@ -627,7 +631,9 @@
       <c r="C9" s="1">
         <v>0</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9" s="1">
         <f>D9-C9</f>
         <v>0</v>
@@ -638,7 +644,9 @@
       <c r="J9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
       <c r="L9" s="1">
         <f>K9-J9</f>
         <v>0</v>
@@ -651,21 +659,25 @@
       <c r="C10" s="1">
         <v>0.1</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>0.1</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:E51" si="0">D10-C10</f>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="J10" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="K10" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="K10" s="1">
+        <v>47</v>
+      </c>
       <c r="L10" s="1">
         <f t="shared" ref="L10:L51" si="1">K10-J10</f>
-        <v>-0.1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
@@ -675,21 +687,25 @@
       <c r="C11" s="1">
         <v>0.2</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>0.2</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
-        <v>0.2</v>
+        <v>100</v>
       </c>
       <c r="J11" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="K11" s="1">
+        <v>92</v>
+      </c>
       <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>-0.2</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
@@ -699,21 +715,25 @@
       <c r="C12" s="1">
         <v>0.3</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.3</v>
+        <v>-1.0000000000000009E-2</v>
       </c>
       <c r="I12" s="1">
-        <v>0.3</v>
+        <v>150</v>
       </c>
       <c r="J12" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="K12" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="K12" s="1">
+        <v>135</v>
+      </c>
       <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>-0.3</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
@@ -723,21 +743,25 @@
       <c r="C13" s="1">
         <v>0.4</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>0.4</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="I13" s="1">
-        <v>0.4</v>
+        <v>200</v>
       </c>
       <c r="J13" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="K13" s="1">
+        <v>183</v>
+      </c>
       <c r="L13" s="1">
         <f t="shared" si="1"/>
-        <v>-0.4</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
@@ -747,21 +771,25 @@
       <c r="C14" s="1">
         <v>0.5</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>0.5</v>
+        <v>250</v>
       </c>
       <c r="J14" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="K14" s="1"/>
+        <v>250</v>
+      </c>
+      <c r="K14" s="1">
+        <v>228</v>
+      </c>
       <c r="L14" s="1">
         <f t="shared" si="1"/>
-        <v>-0.5</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
@@ -771,21 +799,25 @@
       <c r="C15" s="1">
         <v>0.6</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>0.6</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="I15" s="1">
-        <v>0.6</v>
+        <v>300</v>
       </c>
       <c r="J15" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="K15" s="1">
+        <v>277</v>
+      </c>
       <c r="L15" s="1">
         <f t="shared" si="1"/>
-        <v>-0.6</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
@@ -795,999 +827,727 @@
       <c r="C16" s="1">
         <v>0.7</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1">
+        <v>0.68</v>
+      </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>-0.7</v>
+        <v>-1.9999999999999907E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>0.7</v>
+        <v>350</v>
       </c>
       <c r="J16" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="K16" s="1"/>
+        <v>350</v>
+      </c>
+      <c r="K16" s="1">
+        <v>322</v>
+      </c>
       <c r="L16" s="1">
         <f t="shared" si="1"/>
-        <v>-0.7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B17" s="1">
         <v>0.8</v>
       </c>
       <c r="C17" s="1">
         <v>0.8</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>0.79</v>
+      </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>-0.8</v>
+        <v>-1.0000000000000009E-2</v>
       </c>
       <c r="I17" s="1">
-        <v>0.8</v>
+        <v>400</v>
       </c>
       <c r="J17" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K17" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="K17" s="1">
+        <v>370</v>
+      </c>
       <c r="L17" s="1">
         <f t="shared" si="1"/>
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B18" s="1">
         <v>0.9</v>
       </c>
       <c r="C18" s="1">
         <v>0.9</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>0.88</v>
+      </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.9</v>
+        <v>-2.0000000000000018E-2</v>
       </c>
       <c r="I18" s="1">
-        <v>0.9</v>
+        <v>450</v>
       </c>
       <c r="J18" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>450</v>
+      </c>
+      <c r="K18" s="1">
+        <v>413</v>
+      </c>
       <c r="L18" s="1">
         <f t="shared" si="1"/>
-        <v>-0.9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1">
+        <v>0.99</v>
+      </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-1.0000000000000009E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="J19" s="1">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1"/>
+        <v>500</v>
+      </c>
+      <c r="K19" s="1">
+        <v>455</v>
+      </c>
       <c r="L19" s="1">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B20" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="C20" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1">
+        <v>1.08</v>
+      </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="I20" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B21" s="1">
         <v>1.2</v>
       </c>
       <c r="C21" s="1">
         <v>1.2</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1">
+        <v>1.19</v>
+      </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>-1.2</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B22" s="1">
         <v>1.3</v>
       </c>
       <c r="C22" s="1">
         <v>1.3</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>1.28</v>
+      </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>-1.3</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B23" s="1">
         <v>1.4</v>
       </c>
       <c r="C23" s="1">
         <v>1.4</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1">
+        <v>1.37</v>
+      </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>-1.4</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="J23" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B24" s="1">
         <v>1.5</v>
       </c>
       <c r="C24" s="1">
         <v>1.5</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1">
+        <v>1.48</v>
+      </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>-1.5</v>
-      </c>
-      <c r="I24" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B25" s="1">
         <v>1.6</v>
       </c>
       <c r="C25" s="1">
         <v>1.6</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1">
+        <v>1.59</v>
+      </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>-1.6</v>
-      </c>
-      <c r="I25" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="J25" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="K25" s="1"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="1">
+        <f>AVERAGE(L9:L19)</f>
+        <v>-20.727272727272727</v>
+      </c>
       <c r="L25" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+      <c r="M25" s="1" t="str">
+        <f>IF(ABS(K25) &lt; L25, "OK", "FAIL")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B26" s="1">
         <v>1.7</v>
       </c>
       <c r="C26" s="1">
         <v>1.7</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1">
+        <v>1.69</v>
+      </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>-1.7</v>
-      </c>
-      <c r="I26" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="J26" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="K26" s="1"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="1">
+        <f>_xlfn.STDEV.P(L9:L19)</f>
+        <v>13.32182699107616</v>
+      </c>
       <c r="L26" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f>IF(ABS(K26) &lt; L26, "OK", "FAIL")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B27" s="1">
         <v>1.8</v>
       </c>
       <c r="C27" s="1">
         <v>1.8</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1">
+        <v>1.79</v>
+      </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>-1.8</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="K27" s="1"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="1" cm="1">
+        <f t="array" ref="K27">MAX(ABS(L9:L19))</f>
+        <v>45</v>
+      </c>
       <c r="L27" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f>IF(ABS(K27) &lt; L27, "OK", "FAIL")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B28" s="1">
         <v>1.9</v>
       </c>
       <c r="C28" s="1">
         <v>1.9</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1">
+        <v>1.88</v>
+      </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>-1.9</v>
-      </c>
-      <c r="I28" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1">
+        <v>2</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-      <c r="I29" s="1">
-        <v>2</v>
-      </c>
-      <c r="J29" s="1">
-        <v>2</v>
-      </c>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1">
-        <f t="shared" si="1"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B30" s="1">
         <v>2.1</v>
       </c>
       <c r="C30" s="1">
         <v>2.1</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1">
+        <v>2.08</v>
+      </c>
       <c r="E30" s="1">
         <f t="shared" si="0"/>
-        <v>-2.1</v>
-      </c>
-      <c r="I30" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="J30" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B31" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="C31" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1">
+        <v>2.1800000000000002</v>
+      </c>
       <c r="E31" s="1">
         <f t="shared" si="0"/>
-        <v>-2.2000000000000002</v>
-      </c>
-      <c r="I31" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J31" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B32" s="1">
         <v>2.2999999999999998</v>
       </c>
       <c r="C32" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1">
+        <v>2.2799999999999998</v>
+      </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>-2.2999999999999998</v>
-      </c>
-      <c r="I32" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J32" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B33" s="1">
         <v>2.4</v>
       </c>
       <c r="C33" s="1">
         <v>2.4</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1">
+        <v>2.37</v>
+      </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>-2.4</v>
-      </c>
-      <c r="I33" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="J33" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B34" s="1">
         <v>2.5</v>
       </c>
       <c r="C34" s="1">
         <v>2.5</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1">
+        <v>2.48</v>
+      </c>
       <c r="E34" s="1">
         <f t="shared" si="0"/>
-        <v>-2.5</v>
-      </c>
-      <c r="I34" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="J34" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B35" s="1">
         <v>2.6</v>
       </c>
       <c r="C35" s="1">
         <v>2.6</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1">
+        <v>2.57</v>
+      </c>
       <c r="E35" s="1">
         <f t="shared" si="0"/>
-        <v>-2.6</v>
-      </c>
-      <c r="I35" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="J35" s="1">
-        <v>2.6</v>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-3.0000000000000249E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B36" s="1">
         <v>2.7</v>
       </c>
       <c r="C36" s="1">
         <v>2.7</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1">
+        <v>2.67</v>
+      </c>
       <c r="E36" s="1">
         <f t="shared" si="0"/>
-        <v>-2.7</v>
-      </c>
-      <c r="I36" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="J36" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-3.0000000000000249E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B37" s="1">
         <v>2.8</v>
       </c>
       <c r="C37" s="1">
         <v>2.8</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1">
+        <v>2.77</v>
+      </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>-2.8</v>
-      </c>
-      <c r="I37" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="J37" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.8</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B38" s="1">
         <v>2.9</v>
       </c>
       <c r="C38" s="1">
         <v>2.9</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1">
+        <v>2.87</v>
+      </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>-2.9</v>
-      </c>
-      <c r="I38" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="J38" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B39" s="1">
         <v>3</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1">
+        <v>2.97</v>
+      </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-      <c r="I39" s="1">
-        <v>3</v>
-      </c>
-      <c r="J39" s="1">
-        <v>3</v>
-      </c>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1">
-        <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B40" s="1">
         <v>3.1</v>
       </c>
       <c r="C40" s="1">
         <v>3.1</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1">
+        <v>3.08</v>
+      </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>-3.1</v>
-      </c>
-      <c r="I40" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="J40" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B41" s="1">
         <v>3.2</v>
       </c>
       <c r="C41" s="1">
         <v>3.2</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1">
+        <v>3.16</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="0"/>
-        <v>-3.2</v>
-      </c>
-      <c r="I41" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="J41" s="1">
-        <v>3.2</v>
-      </c>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B42" s="1">
         <v>3.3</v>
       </c>
       <c r="C42" s="1">
         <v>3.3</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1">
+        <v>3.25</v>
+      </c>
       <c r="E42" s="1">
         <f t="shared" si="0"/>
-        <v>-3.3</v>
-      </c>
-      <c r="I42" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="J42" s="1">
-        <v>3.3</v>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-4.9999999999999822E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B43" s="1">
         <v>3.4</v>
       </c>
       <c r="C43" s="1">
         <v>3.4</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1">
+        <v>3.36</v>
+      </c>
       <c r="E43" s="1">
         <f t="shared" si="0"/>
-        <v>-3.4</v>
-      </c>
-      <c r="I43" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="J43" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.4</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B44" s="1">
         <v>3.5</v>
       </c>
       <c r="C44" s="1">
         <v>3.5</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1">
+        <v>3.47</v>
+      </c>
       <c r="E44" s="1">
         <f t="shared" si="0"/>
-        <v>-3.5</v>
-      </c>
-      <c r="I44" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="J44" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B45" s="1">
         <v>3.6</v>
       </c>
       <c r="C45" s="1">
         <v>3.6</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1">
+        <v>3.57</v>
+      </c>
       <c r="E45" s="1">
         <f t="shared" si="0"/>
-        <v>-3.6</v>
-      </c>
-      <c r="I45" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="J45" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-3.0000000000000249E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B46" s="1">
         <v>3.7</v>
       </c>
       <c r="C46" s="1">
         <v>3.7</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1">
+        <v>3.66</v>
+      </c>
       <c r="E46" s="1">
         <f t="shared" si="0"/>
-        <v>-3.7</v>
-      </c>
-      <c r="I46" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="J46" s="1">
-        <v>3.7</v>
-      </c>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.7</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B47" s="1">
         <v>3.8</v>
       </c>
       <c r="C47" s="1">
         <v>3.8</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1">
+        <v>3.76</v>
+      </c>
       <c r="E47" s="1">
         <f t="shared" si="0"/>
-        <v>-3.8</v>
-      </c>
-      <c r="I47" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="J47" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.8</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B48" s="1">
         <v>3.9</v>
       </c>
       <c r="C48" s="1">
         <v>3.9</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1">
+        <v>3.87</v>
+      </c>
       <c r="E48" s="1">
         <f t="shared" si="0"/>
-        <v>-3.9</v>
-      </c>
-      <c r="I48" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="J48" s="1">
-        <v>3.9</v>
-      </c>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.9</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
+        <v>-2.9999999999999805E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B49" s="1">
         <v>4</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1">
+        <v>3.96</v>
+      </c>
       <c r="E49" s="1">
         <f t="shared" si="0"/>
-        <v>-4</v>
-      </c>
-      <c r="I49" s="1">
-        <v>4</v>
-      </c>
-      <c r="J49" s="1">
-        <v>4</v>
-      </c>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1">
-        <f t="shared" si="1"/>
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B50" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="C50" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1">
+        <v>4.0599999999999996</v>
+      </c>
       <c r="E50" s="1">
         <f t="shared" si="0"/>
-        <v>-4.0999999999999996</v>
-      </c>
-      <c r="I50" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J50" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1">
-        <f t="shared" si="1"/>
-        <v>-4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B51" s="1">
         <v>4.2</v>
       </c>
       <c r="C51" s="1">
         <v>4.2</v>
       </c>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1">
+        <v>4.16</v>
+      </c>
       <c r="E51" s="1">
         <f t="shared" si="0"/>
-        <v>-4.2</v>
-      </c>
-      <c r="I51" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="J51" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1">
-        <f t="shared" si="1"/>
-        <v>-4.2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.45">
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B53" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C53" s="7"/>
-      <c r="D53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" s="7"/>
-      <c r="K53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="D53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B54" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="1">
         <f>AVERAGE(E9:E51)</f>
-        <v>-2.1</v>
+        <v>-2.1395348837209293E-2</v>
       </c>
       <c r="E54" s="1">
         <v>0.05</v>
       </c>
       <c r="F54" s="1" t="str">
         <f>IF(ABS(D54) &lt; E54, "OK", "FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J54" s="7"/>
-      <c r="K54" s="1">
-        <f>AVERAGE(L9:L51)</f>
-        <v>-2.1</v>
-      </c>
-      <c r="L54" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="M54" s="1" t="str">
-        <f>IF(ABS(K54) &lt; L54, "OK", "FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.45">
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B55" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="1">
         <f>_xlfn.STDEV.P(E9:E51)</f>
-        <v>1.240967364599086</v>
+        <v>1.3738656267666908E-2</v>
       </c>
       <c r="E55" s="1">
         <v>0.1</v>
       </c>
       <c r="F55" s="1" t="str">
         <f>IF(ABS(D55) &lt; E55, "OK", "FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J55" s="7"/>
-      <c r="K55" s="1">
-        <f>_xlfn.STDEV.P(L9:L51)</f>
-        <v>1.240967364599086</v>
-      </c>
-      <c r="L55" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="M55" s="1" t="str">
-        <f>IF(ABS(K55) &lt; L55, "OK", "FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.45">
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B56" s="6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="1" cm="1">
         <f t="array" ref="D56">MAX(ABS(E9:E51))</f>
-        <v>4.2</v>
+        <v>4.9999999999999822E-2</v>
       </c>
       <c r="E56" s="1">
         <v>0.2</v>
       </c>
       <c r="F56" s="1" t="str">
         <f>IF(ABS(D56) &lt; E56, "OK", "FAIL")</f>
-        <v>FAIL</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J56" s="7"/>
-      <c r="K56" s="1" cm="1">
-        <f t="array" ref="K56">MAX(ABS(L9:L51))</f>
-        <v>4.2</v>
-      </c>
-      <c r="L56" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="M56" s="1" t="str">
-        <f>IF(ABS(K56) &lt; L56, "OK", "FAIL")</f>
-        <v>FAIL</v>
+        <v>OK</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
   </mergeCells>
   <conditionalFormatting sqref="F54:F56">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
@@ -1797,7 +1557,7 @@
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M54:M56">
+  <conditionalFormatting sqref="M25:M27">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -1807,4 +1567,10 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{15ce9348-be2a-462b-8fc0-e1765a9b204a}" enabled="0" method="" siteId="{15ce9348-be2a-462b-8fc0-e1765a9b204a}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>